<commit_message>
week 6 functional requirements user stories
</commit_message>
<xml_diff>
--- a/BusinessDocuments/_W6_Functional Requirements_User Stories.xlsx
+++ b/BusinessDocuments/_W6_Functional Requirements_User Stories.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunco\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunco\Google Drive (scottsun17@gmail.com)\Computer Science Project\BundleBid\BusinessDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2640B3A-2771-438D-AD7F-7F97B07F8D68}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E352ADD-DEDF-4370-90E9-44EEA9E14166}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="168">
   <si>
     <t>As a/an</t>
   </si>
@@ -370,9 +370,6 @@
     <t>02.03 Close Account</t>
   </si>
   <si>
-    <t>02.04 Purchase History</t>
-  </si>
-  <si>
     <t>02.05 Sign in to Account</t>
   </si>
   <si>
@@ -521,6 +518,18 @@
   </si>
   <si>
     <t>mark the payment is verified and completed</t>
+  </si>
+  <si>
+    <t>02.04 Bidding History</t>
+  </si>
+  <si>
+    <t>01.04 Listing History</t>
+  </si>
+  <si>
+    <t>access the history of item sold</t>
+  </si>
+  <si>
+    <t>see my sell's history</t>
   </si>
 </sst>
 </file>
@@ -585,7 +594,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -634,8 +643,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -835,30 +850,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -889,6 +880,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -900,7 +928,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1005,6 +1033,59 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1031,40 +1112,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1412,10 +1459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E925F31-0E3F-4047-8350-B0EF6A0D6BDC}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView zoomScale="61" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="61" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1427,6 +1474,7 @@
     <col min="5" max="5" width="48.296875" customWidth="1"/>
     <col min="6" max="6" width="50.09765625" customWidth="1"/>
     <col min="7" max="7" width="12.296875" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="11" style="40"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.7">
@@ -1440,7 +1488,7 @@
       <c r="F1" s="3"/>
       <c r="G1" s="13"/>
     </row>
-    <row r="2" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1449,316 +1497,368 @@
       <c r="F2" s="3"/>
       <c r="G2" s="13"/>
     </row>
-    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="49" t="s">
+    <row r="3" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+      <c r="A3" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="50" t="s">
+      <c r="E3" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="51" t="s">
+      <c r="F3" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="50" t="s">
+      <c r="G3" s="42" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="56" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="52"/>
-      <c r="B4" s="53" t="s">
+    <row r="4" spans="1:7" s="41" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="D4" s="45" t="s">
+        <v>130</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="F4" s="47" t="s">
+        <v>135</v>
+      </c>
+      <c r="G4" s="48"/>
+    </row>
+    <row r="5" spans="1:7" s="41" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" s="49" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="F5" s="50" t="s">
+        <v>137</v>
+      </c>
+      <c r="G5" s="9"/>
+    </row>
+    <row r="6" spans="1:7" s="41" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" s="49" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="F6" s="50" t="s">
+        <v>139</v>
+      </c>
+      <c r="G6" s="9"/>
+    </row>
+    <row r="7" spans="1:7" s="41" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" s="49" t="s">
+        <v>165</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="F7" s="50" t="s">
+        <v>167</v>
+      </c>
+      <c r="G7" s="9"/>
+    </row>
+    <row r="8" spans="1:7" s="41" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" s="55" t="s">
         <v>123</v>
       </c>
-      <c r="C4" s="54" t="s">
-        <v>108</v>
-      </c>
-      <c r="D4" s="53" t="s">
+      <c r="C8" s="56" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="55" t="s">
+        <v>127</v>
+      </c>
+      <c r="E8" s="55" t="s">
+        <v>140</v>
+      </c>
+      <c r="F8" s="57" t="s">
+        <v>141</v>
+      </c>
+      <c r="G8" s="58"/>
+    </row>
+    <row r="9" spans="1:7" s="41" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="55" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" s="56" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" s="55" t="s">
         <v>131</v>
       </c>
-      <c r="E4" s="53" t="s">
-        <v>135</v>
-      </c>
-      <c r="F4" s="53" t="s">
-        <v>136</v>
-      </c>
-      <c r="G4" s="55"/>
-    </row>
-    <row r="5" spans="1:7" s="56" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="52"/>
-      <c r="B5" s="53" t="s">
+      <c r="E9" s="55" t="s">
+        <v>142</v>
+      </c>
+      <c r="F9" s="57" t="s">
+        <v>143</v>
+      </c>
+      <c r="G9" s="58"/>
+    </row>
+    <row r="10" spans="1:7" s="41" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10" s="55" t="s">
         <v>123</v>
       </c>
-      <c r="C5" s="54" t="s">
-        <v>109</v>
-      </c>
-      <c r="D5" s="53" t="s">
+      <c r="C10" s="56" t="s">
+        <v>113</v>
+      </c>
+      <c r="D10" s="55" t="s">
+        <v>131</v>
+      </c>
+      <c r="E10" s="55" t="s">
+        <v>144</v>
+      </c>
+      <c r="F10" s="57" t="s">
+        <v>145</v>
+      </c>
+      <c r="G10" s="58"/>
+    </row>
+    <row r="11" spans="1:7" s="41" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C11" s="49" t="s">
+        <v>164</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="F11" s="50" t="s">
+        <v>149</v>
+      </c>
+      <c r="G11" s="9"/>
+    </row>
+    <row r="12" spans="1:7" s="41" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" s="55" t="s">
+        <v>123</v>
+      </c>
+      <c r="C12" s="56" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" s="55" t="s">
         <v>128</v>
       </c>
-      <c r="E5" s="53" t="s">
-        <v>137</v>
-      </c>
-      <c r="F5" s="53" t="s">
-        <v>138</v>
-      </c>
-      <c r="G5" s="55"/>
-    </row>
-    <row r="6" spans="1:7" s="56" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="52"/>
-      <c r="B6" s="53" t="s">
-        <v>123</v>
-      </c>
-      <c r="C6" s="54" t="s">
-        <v>110</v>
-      </c>
-      <c r="D6" s="53" t="s">
-        <v>131</v>
-      </c>
-      <c r="E6" s="53" t="s">
-        <v>139</v>
-      </c>
-      <c r="F6" s="53" t="s">
-        <v>140</v>
-      </c>
-      <c r="G6" s="55"/>
-    </row>
-    <row r="7" spans="1:7" s="56" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="52"/>
-      <c r="B7" s="53" t="s">
+      <c r="E12" s="55" t="s">
+        <v>147</v>
+      </c>
+      <c r="F12" s="57" t="s">
+        <v>146</v>
+      </c>
+      <c r="G12" s="58"/>
+    </row>
+    <row r="13" spans="1:7" s="41" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="C7" s="54" t="s">
-        <v>111</v>
-      </c>
-      <c r="D7" s="53" t="s">
+      <c r="C13" s="49" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="F13" s="50" t="s">
+        <v>151</v>
+      </c>
+      <c r="G13" s="9"/>
+    </row>
+    <row r="14" spans="1:7" s="41" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C14" s="49" t="s">
+        <v>116</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="F14" s="50" t="s">
+        <v>153</v>
+      </c>
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="1:7" s="41" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C15" s="49" t="s">
+        <v>117</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="F15" s="50" t="s">
+        <v>155</v>
+      </c>
+      <c r="G15" s="9"/>
+    </row>
+    <row r="16" spans="1:7" s="41" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C16" s="49" t="s">
+        <v>118</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="F16" s="50" t="s">
+        <v>157</v>
+      </c>
+      <c r="G16" s="9"/>
+    </row>
+    <row r="17" spans="1:7" s="41" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C17" s="51" t="s">
+        <v>119</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="F17" s="50" t="s">
+        <v>159</v>
+      </c>
+      <c r="G17" s="9"/>
+    </row>
+    <row r="18" spans="1:7" s="41" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C18" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="E7" s="53" t="s">
-        <v>141</v>
-      </c>
-      <c r="F7" s="53" t="s">
-        <v>142</v>
-      </c>
-      <c r="G7" s="55"/>
-    </row>
-    <row r="8" spans="1:7" s="56" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="52"/>
-      <c r="B8" s="53" t="s">
-        <v>124</v>
-      </c>
-      <c r="C8" s="54" t="s">
-        <v>112</v>
-      </c>
-      <c r="D8" s="53" t="s">
-        <v>132</v>
-      </c>
-      <c r="E8" s="53" t="s">
-        <v>143</v>
-      </c>
-      <c r="F8" s="53" t="s">
-        <v>144</v>
-      </c>
-      <c r="G8" s="55"/>
-    </row>
-    <row r="9" spans="1:7" s="56" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="52"/>
-      <c r="B9" s="53" t="s">
-        <v>124</v>
-      </c>
-      <c r="C9" s="54" t="s">
-        <v>113</v>
-      </c>
-      <c r="D9" s="53" t="s">
-        <v>132</v>
-      </c>
-      <c r="E9" s="53" t="s">
-        <v>145</v>
-      </c>
-      <c r="F9" s="53" t="s">
-        <v>146</v>
-      </c>
-      <c r="G9" s="55"/>
-    </row>
-    <row r="10" spans="1:7" s="56" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="52"/>
-      <c r="B10" s="53" t="s">
-        <v>124</v>
-      </c>
-      <c r="C10" s="54" t="s">
-        <v>114</v>
-      </c>
-      <c r="D10" s="53" t="s">
+      <c r="E18" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="F18" s="53" t="s">
+        <v>161</v>
+      </c>
+      <c r="G18" s="9"/>
+    </row>
+    <row r="19" spans="1:7" s="41" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C19" s="52" t="s">
+        <v>121</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="E10" s="53" t="s">
-        <v>149</v>
-      </c>
-      <c r="F10" s="53" t="s">
-        <v>150</v>
-      </c>
-      <c r="G10" s="55"/>
-    </row>
-    <row r="11" spans="1:7" s="56" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="52"/>
-      <c r="B11" s="53" t="s">
-        <v>124</v>
-      </c>
-      <c r="C11" s="54" t="s">
-        <v>115</v>
-      </c>
-      <c r="D11" s="53" t="s">
-        <v>129</v>
-      </c>
-      <c r="E11" s="53" t="s">
-        <v>148</v>
-      </c>
-      <c r="F11" s="53" t="s">
-        <v>147</v>
-      </c>
-      <c r="G11" s="55"/>
-    </row>
-    <row r="12" spans="1:7" s="56" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="52"/>
-      <c r="B12" s="53" t="s">
-        <v>125</v>
-      </c>
-      <c r="C12" s="54" t="s">
-        <v>116</v>
-      </c>
-      <c r="D12" s="53" t="s">
-        <v>130</v>
-      </c>
-      <c r="E12" s="53" t="s">
-        <v>151</v>
-      </c>
-      <c r="F12" s="53" t="s">
-        <v>152</v>
-      </c>
-      <c r="G12" s="55"/>
-    </row>
-    <row r="13" spans="1:7" s="56" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="52"/>
-      <c r="B13" s="53" t="s">
-        <v>125</v>
-      </c>
-      <c r="C13" s="54" t="s">
-        <v>117</v>
-      </c>
-      <c r="D13" s="53" t="s">
-        <v>130</v>
-      </c>
-      <c r="E13" s="53" t="s">
-        <v>153</v>
-      </c>
-      <c r="F13" s="53" t="s">
-        <v>154</v>
-      </c>
-      <c r="G13" s="55"/>
-    </row>
-    <row r="14" spans="1:7" s="56" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="52"/>
-      <c r="B14" s="53" t="s">
-        <v>125</v>
-      </c>
-      <c r="C14" s="54" t="s">
-        <v>118</v>
-      </c>
-      <c r="D14" s="53" t="s">
-        <v>130</v>
-      </c>
-      <c r="E14" s="53" t="s">
-        <v>155</v>
-      </c>
-      <c r="F14" s="53" t="s">
-        <v>156</v>
-      </c>
-      <c r="G14" s="55"/>
-    </row>
-    <row r="15" spans="1:7" s="56" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="57"/>
-      <c r="B15" s="53" t="s">
-        <v>126</v>
-      </c>
-      <c r="C15" s="54" t="s">
-        <v>119</v>
-      </c>
-      <c r="D15" s="53" t="s">
-        <v>130</v>
-      </c>
-      <c r="E15" s="53" t="s">
-        <v>157</v>
-      </c>
-      <c r="F15" s="53" t="s">
-        <v>158</v>
-      </c>
-      <c r="G15" s="55"/>
-    </row>
-    <row r="16" spans="1:7" s="56" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="52"/>
-      <c r="B16" s="53" t="s">
-        <v>126</v>
-      </c>
-      <c r="C16" s="58" t="s">
-        <v>120</v>
-      </c>
-      <c r="D16" s="53" t="s">
-        <v>130</v>
-      </c>
-      <c r="E16" s="53" t="s">
-        <v>159</v>
-      </c>
-      <c r="F16" s="53" t="s">
-        <v>160</v>
-      </c>
-      <c r="G16" s="55"/>
-    </row>
-    <row r="17" spans="1:7" s="56" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="52"/>
-      <c r="B17" s="53" t="s">
-        <v>127</v>
-      </c>
-      <c r="C17" s="59" t="s">
-        <v>121</v>
-      </c>
-      <c r="D17" s="53" t="s">
-        <v>129</v>
-      </c>
-      <c r="E17" s="60" t="s">
-        <v>161</v>
-      </c>
-      <c r="F17" s="60" t="s">
+      <c r="E19" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="G17" s="55"/>
-    </row>
-    <row r="18" spans="1:7" s="56" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="52"/>
-      <c r="B18" s="53" t="s">
-        <v>127</v>
-      </c>
-      <c r="C18" s="59" t="s">
-        <v>122</v>
-      </c>
-      <c r="D18" s="53" t="s">
-        <v>134</v>
-      </c>
-      <c r="E18" s="60" t="s">
+      <c r="F19" s="53" t="s">
         <v>163</v>
       </c>
-      <c r="F18" s="60" t="s">
-        <v>164</v>
-      </c>
-      <c r="G18" s="55"/>
+      <c r="G19" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1766,8 +1866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AX31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView topLeftCell="A2" zoomScale="65" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1825,7 +1925,7 @@
       </c>
     </row>
     <row r="4" spans="1:50" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="62" t="s">
         <v>105</v>
       </c>
       <c r="B4" s="38" t="s">
@@ -1846,7 +1946,7 @@
       <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="44"/>
+      <c r="A5" s="63"/>
       <c r="B5" s="10" t="s">
         <v>51</v>
       </c>
@@ -1908,7 +2008,7 @@
       <c r="AX5" s="5"/>
     </row>
     <row r="6" spans="1:50" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="44"/>
+      <c r="A6" s="63"/>
       <c r="B6" s="17" t="s">
         <v>51</v>
       </c>
@@ -1927,7 +2027,7 @@
       <c r="G6" s="20"/>
     </row>
     <row r="7" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="44"/>
+      <c r="A7" s="63"/>
       <c r="B7" s="18" t="s">
         <v>51</v>
       </c>
@@ -1989,7 +2089,7 @@
       <c r="AX7" s="5"/>
     </row>
     <row r="8" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="44"/>
+      <c r="A8" s="63"/>
       <c r="B8" s="18" t="s">
         <v>51</v>
       </c>
@@ -2051,7 +2151,7 @@
       <c r="AX8" s="5"/>
     </row>
     <row r="9" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="44"/>
+      <c r="A9" s="63"/>
       <c r="B9" s="18" t="s">
         <v>51</v>
       </c>
@@ -2113,7 +2213,7 @@
       <c r="AX9" s="5"/>
     </row>
     <row r="10" spans="1:50" s="4" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="44"/>
+      <c r="A10" s="63"/>
       <c r="B10" s="18" t="s">
         <v>51</v>
       </c>
@@ -2175,7 +2275,7 @@
       <c r="AX10" s="5"/>
     </row>
     <row r="11" spans="1:50" s="4" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="44"/>
+      <c r="A11" s="63"/>
       <c r="B11" s="18" t="s">
         <v>51</v>
       </c>
@@ -2237,7 +2337,7 @@
       <c r="AX11" s="5"/>
     </row>
     <row r="12" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="44"/>
+      <c r="A12" s="63"/>
       <c r="B12" s="18" t="s">
         <v>51</v>
       </c>
@@ -2299,7 +2399,7 @@
       <c r="AX12" s="5"/>
     </row>
     <row r="13" spans="1:50" s="4" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="44"/>
+      <c r="A13" s="63"/>
       <c r="B13" s="22" t="s">
         <v>51</v>
       </c>
@@ -2361,7 +2461,7 @@
       <c r="AX13" s="5"/>
     </row>
     <row r="14" spans="1:50" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="45"/>
+      <c r="A14" s="64"/>
       <c r="B14" s="18" t="s">
         <v>51</v>
       </c>
@@ -2444,7 +2544,7 @@
       <c r="AX15" s="5"/>
     </row>
     <row r="16" spans="1:50" s="1" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="65" t="s">
         <v>105</v>
       </c>
       <c r="B16" s="18" t="s">
@@ -2508,7 +2608,7 @@
       <c r="AX16" s="5"/>
     </row>
     <row r="17" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="44"/>
+      <c r="A17" s="63"/>
       <c r="B17" s="18" t="s">
         <v>56</v>
       </c>
@@ -2527,7 +2627,7 @@
       <c r="G17" s="20"/>
     </row>
     <row r="18" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="45"/>
+      <c r="A18" s="64"/>
       <c r="B18" s="18" t="s">
         <v>56</v>
       </c>
@@ -2546,7 +2646,7 @@
       <c r="G18" s="20"/>
     </row>
     <row r="19" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="59" t="s">
         <v>106</v>
       </c>
       <c r="B19" s="26" t="s">
@@ -2567,7 +2667,7 @@
       <c r="G19" s="33"/>
     </row>
     <row r="20" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="41"/>
+      <c r="A20" s="60"/>
       <c r="B20" s="26" t="s">
         <v>70</v>
       </c>
@@ -2586,7 +2686,7 @@
       <c r="G20" s="33"/>
     </row>
     <row r="21" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="42"/>
+      <c r="A21" s="61"/>
       <c r="B21" s="26" t="s">
         <v>70</v>
       </c>
@@ -2605,7 +2705,7 @@
       <c r="G21" s="33"/>
     </row>
     <row r="22" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="47" t="s">
+      <c r="A22" s="66" t="s">
         <v>106</v>
       </c>
       <c r="B22" s="11" t="s">
@@ -2626,7 +2726,7 @@
       <c r="G22" s="37"/>
     </row>
     <row r="23" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="48"/>
+      <c r="A23" s="67"/>
       <c r="B23" s="11" t="s">
         <v>71</v>
       </c>
@@ -2645,7 +2745,7 @@
       <c r="G23" s="37"/>
     </row>
     <row r="24" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="40" t="s">
+      <c r="A24" s="59" t="s">
         <v>106</v>
       </c>
       <c r="B24" s="26" t="s">
@@ -2666,7 +2766,7 @@
       <c r="G24" s="33"/>
     </row>
     <row r="25" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="42"/>
+      <c r="A25" s="61"/>
       <c r="B25" s="26" t="s">
         <v>72</v>
       </c>
@@ -2685,7 +2785,7 @@
       <c r="G25" s="33"/>
     </row>
     <row r="26" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="40" t="s">
+      <c r="A26" s="59" t="s">
         <v>106</v>
       </c>
       <c r="B26" s="26" t="s">
@@ -2706,7 +2806,7 @@
       <c r="G26" s="33"/>
     </row>
     <row r="27" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="42"/>
+      <c r="A27" s="61"/>
       <c r="B27" s="26" t="s">
         <v>73</v>
       </c>
@@ -2725,7 +2825,7 @@
       <c r="G27" s="33"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="40" t="s">
+      <c r="A28" s="59" t="s">
         <v>106</v>
       </c>
       <c r="B28" s="30" t="s">
@@ -2746,7 +2846,7 @@
       <c r="G28" s="33"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="41"/>
+      <c r="A29" s="60"/>
       <c r="B29" s="30" t="s">
         <v>74</v>
       </c>
@@ -2765,7 +2865,7 @@
       <c r="G29" s="33"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="41"/>
+      <c r="A30" s="60"/>
       <c r="B30" s="30" t="s">
         <v>74</v>
       </c>
@@ -2784,7 +2884,7 @@
       <c r="G30" s="33"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="42"/>
+      <c r="A31" s="61"/>
       <c r="B31" s="30" t="s">
         <v>74</v>
       </c>

</xml_diff>